<commit_message>
V1.3 multi language support addition
</commit_message>
<xml_diff>
--- a/jinding_config_build/tmp_V13/relation.xlsx
+++ b/jinding_config_build/tmp_V13/relation.xlsx
@@ -17,6 +17,7 @@
     <sheet name="dependence" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="independence" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="reset" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="language" sheetId="10" state="visible" r:id="rId11"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -1654,7 +1655,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="80">
   <si>
     <t xml:space="preserve">可选功能</t>
   </si>
@@ -1808,6 +1809,12 @@
     <t xml:space="preserve">场景/功能</t>
   </si>
   <si>
+    <t xml:space="preserve">凉风</t>
+  </si>
+  <si>
+    <t xml:space="preserve">凉风扇</t>
+  </si>
+  <si>
     <t xml:space="preserve">开</t>
   </si>
   <si>
@@ -1833,6 +1840,69 @@
   </si>
   <si>
     <t xml:space="preserve">关</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ori</t>
+  </si>
+  <si>
+    <t xml:space="preserve">en</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scene_bath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scene_brush</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scene_venti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wind_speed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">air_change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cool_wind_inner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cool_drying</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hot_drying</t>
+  </si>
+  <si>
+    <t xml:space="preserve">swing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">timer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">light1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">light2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">music_play</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cool_fan_outside</t>
+  </si>
+  <si>
+    <t xml:space="preserve">neg_ion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">air_detection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">power</t>
+  </si>
+  <si>
+    <t xml:space="preserve">go_away</t>
   </si>
 </sst>
 </file>
@@ -1842,7 +1912,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1889,6 +1959,13 @@
     <font>
       <b val="true"/>
       <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Noto Sans CJK SC Regular"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Noto Sans CJK SC Regular"/>
       <family val="2"/>
@@ -2006,7 +2083,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2099,6 +2176,18 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -2179,16 +2268,16 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="1" sqref="G14 H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.45"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.4279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="2" style="1" width="13.4139534883721"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="14.8883720930233"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="78.2697674418605"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="13.5348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.9209302325581"/>
+    <col collapsed="false" hidden="false" max="6" min="2" style="1" width="14.153488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="15.6279069767442"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="83.0651162790698"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="14.2744186046512"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2291,6 +2380,207 @@
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B32"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C27" activeCellId="1" sqref="G14 C27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.5023255813953"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3767441860465"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.5023255813953"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,标准"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,标准"&amp;12页 &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -2307,15 +2597,15 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="J12" activeCellId="0" sqref="J12"/>
+      <selection pane="bottomRight" activeCell="J12" activeCellId="1" sqref="G14 J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="33.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.7348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.0279069767442"/>
-    <col collapsed="false" hidden="false" max="25" min="3" style="1" width="14.153488372093"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="1" width="11.8139534883721"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.7209302325581"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.2604651162791"/>
+    <col collapsed="false" hidden="false" max="25" min="3" style="1" width="14.8883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="1" width="12.4279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4154,12 +4444,12 @@
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K21" activeCellId="0" sqref="K21"/>
+      <selection pane="topLeft" activeCell="K21" activeCellId="1" sqref="G14 K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4884,13 +5174,13 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.8139534883721"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="12.4279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.9209302325581"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="12.9209302325581"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4913,10 +5203,10 @@
         <v>7</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4924,19 +5214,19 @@
         <v>2</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>36</v>
@@ -4950,19 +5240,19 @@
         <v>10</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>46</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>46</v>
@@ -4976,13 +5266,13 @@
         <v>12</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>46</v>
@@ -5016,18 +5306,18 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F34" activeCellId="0" sqref="F34"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="G14 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.7813953488372"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.0139534883721"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>6</v>
@@ -5036,7 +5326,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>25</v>
@@ -5087,7 +5377,7 @@
     </row>
     <row r="4" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>46</v>
@@ -5164,18 +5454,18 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="G14 B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.553488372093"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="12.4279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.5348837209302"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="12.9209302325581"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="16" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>28</v>
@@ -5184,10 +5474,10 @@
         <v>27</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5195,13 +5485,13 @@
         <v>6</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>46</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E2" s="18" t="n">
         <v>28</v>
@@ -5215,10 +5505,10 @@
         <v>46</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E3" s="19" t="s">
         <v>46</v>
@@ -5226,7 +5516,7 @@
     </row>
     <row r="4" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="17" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>36</v>
@@ -5235,7 +5525,7 @@
         <v>36</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E4" s="19" t="s">
         <v>46</v>
@@ -5294,18 +5584,18 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="1" sqref="G14 C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.553488372093"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="12.4279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.5348837209302"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="12.9209302325581"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="16" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>28</v>
@@ -5314,10 +5604,10 @@
         <v>27</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5356,7 +5646,7 @@
     </row>
     <row r="4" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="17" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>36</v>
@@ -5424,13 +5714,13 @@
   <dimension ref="A1:H65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="G14 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1023" min="1" style="20" width="11.5674418604651"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="1023" min="1" style="20" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5444,7 +5734,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="E1" s="21" t="s">
         <v>29</v>
@@ -5480,12 +5770,12 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L19" activeCellId="0" sqref="L19"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="G14 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="12.6744186046512"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>